<commit_message>
make circuit schema by KiCad
</commit_message>
<xml_diff>
--- a/config_PIC24FJ64GB002_UsbStudy_02.xlsx
+++ b/config_PIC24FJ64GB002_UsbStudy_02.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mura01\Google ドライブ\PIC24F\20190829_USBMSCtest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEAD4E13-9F12-4A65-AE28-39E521A7173A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A4B12A-05B3-45E2-94DD-6039CEBB1555}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1305" yWindow="480" windowWidth="24900" windowHeight="15120" tabRatio="500" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="120" windowWidth="17895" windowHeight="12720" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CPU" sheetId="1" r:id="rId1"/>
@@ -450,7 +450,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="946">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="991">
   <si>
     <t>CPU</t>
   </si>
@@ -4001,6 +4001,168 @@
     <t>bits/sec</t>
     <phoneticPr fontId="8"/>
   </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t>0x00,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x05,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x01,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x00,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x00</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x09,</t>
+  </si>
+  <si>
+    <t>USB アドレス設定コマンド。　アドレス 1 に設定（赤字の部分）</t>
+    <rPh sb="8" eb="10">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>アカジ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>ブブン</t>
+    </rPh>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>USB Config設定コマンド。　Config 1 に設定(赤字の部分）</t>
+    <rPh sb="10" eb="12">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>アカジ</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>ブブン</t>
+    </rPh>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>bmRequestType</t>
+  </si>
+  <si>
+    <t>bRequest</t>
+  </si>
+  <si>
+    <t>wValue</t>
+  </si>
+  <si>
+    <t>wIndex</t>
+  </si>
+  <si>
+    <t>wLength</t>
+  </si>
+  <si>
+    <t>*wValue,wIndex,wLengthは、リトルエンディアン。0x1234は、0x34 0x12の順となる。</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>bmRequestTypeはビットマップ形式であり、各ビットの意味は以下の通り。</t>
+  </si>
+  <si>
+    <t>D7: Data transfer direction</t>
+  </si>
+  <si>
+    <t>0 = Host-to-device</t>
+  </si>
+  <si>
+    <t>1 = Device-to-host</t>
+  </si>
+  <si>
+    <t>D6-D5: Type</t>
+  </si>
+  <si>
+    <t>0 = Standard</t>
+  </si>
+  <si>
+    <t>1 = Class</t>
+  </si>
+  <si>
+    <t>2 = Vendor</t>
+  </si>
+  <si>
+    <t>3 = Reserved</t>
+  </si>
+  <si>
+    <t>D4-D0: Recipient</t>
+  </si>
+  <si>
+    <t>0 = Device</t>
+  </si>
+  <si>
+    <t>1 = Interface</t>
+  </si>
+  <si>
+    <t>2 = Endpoint</t>
+  </si>
+  <si>
+    <t>3 = Other</t>
+  </si>
+  <si>
+    <t>4…31 = Reserved</t>
+  </si>
+  <si>
+    <t>bRequestの値は次の通り。</t>
+  </si>
+  <si>
+    <t>0 = GET_STATUS</t>
+  </si>
+  <si>
+    <t>1 = CLEAR_FEATURE</t>
+  </si>
+  <si>
+    <t>2 = Reserved for future use</t>
+  </si>
+  <si>
+    <t>3 = SET_FEATURE</t>
+  </si>
+  <si>
+    <t>4 = Reserved for future use</t>
+  </si>
+  <si>
+    <t>5 = SET_ADDRESS</t>
+  </si>
+  <si>
+    <t>6 = GET_DESCRIPTOR</t>
+  </si>
+  <si>
+    <t>7 = SET_DESCRIPTOR</t>
+  </si>
+  <si>
+    <t>8 = GET_CONFIGURATION</t>
+  </si>
+  <si>
+    <t>9 = SET_CONFIGURATION</t>
+  </si>
+  <si>
+    <t>10 = GET_INTERFACE</t>
+  </si>
+  <si>
+    <t>11 = SET_INTERFACE</t>
+  </si>
+  <si>
+    <t>12 = SYNCH_FRAME</t>
+  </si>
 </sst>
 </file>
 
@@ -4012,7 +4174,7 @@
     <numFmt numFmtId="178" formatCode="#,##0.000_ "/>
     <numFmt numFmtId="179" formatCode="#,##0.0000_ "/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -4073,6 +4235,13 @@
     </font>
     <font>
       <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
@@ -4433,7 +4602,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4626,6 +4795,17 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="178" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="176" fontId="0" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7958,6 +8138,50 @@
         <a:ln>
           <a:noFill/>
         </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>507690</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>163810</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{297AEA62-4AFB-4881-935F-C21CA877C7A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10498667" y="2370667"/>
+          <a:ext cx="2476190" cy="1857143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -10316,15 +10540,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>529166</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>141112</xdr:rowOff>
+      <xdr:colOff>542772</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>108857</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>153728</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>26643</xdr:rowOff>
+      <xdr:colOff>167334</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>149107</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -10339,8 +10563,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5221110" y="8607779"/>
-          <a:ext cx="4986785" cy="1473031"/>
+          <a:off x="5210022" y="9837964"/>
+          <a:ext cx="4958562" cy="1809179"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10371,8 +10595,9 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>　U1ADDR</a:t>
@@ -10380,38 +10605,40 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>　　USB</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>デバイスに割振ったアドレスを指定 </a:t>
+            <a:t>デバイスに割振ったアドレスを指定</a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>= 1</a:t>
-          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1200" b="0" strike="noStrike" spc="-1">
+            <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>　</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1200" b="0" strike="noStrike" spc="-1">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>U1BDTP1</a:t>
@@ -10419,56 +10646,119 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1200" b="0" strike="noStrike" spc="-1">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t> </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1200" b="0">
               <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>　　BDT</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1200" b="0">
               <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>テーブルの上位</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1200" b="0">
               <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>7BITS</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0">
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1200" b="0">
               <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>のアドレスを格納</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1100" b="0" strike="noStrike" spc="-1">
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1200" b="0">
+            <a:effectLst/>
+            <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="ja-JP" sz="1200" b="0">
+              <a:effectLst/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>　</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1200" b="0">
+              <a:effectLst/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>U1CON</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1200">
+            <a:effectLst/>
+            <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1200" b="0">
+              <a:effectLst/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>　</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="ja-JP" sz="1200" b="0">
+              <a:effectLst/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>　</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1200" b="0">
+              <a:effectLst/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>SOFEN=1:SOF packet の自動1ms送信スタート</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1200">
+            <a:effectLst/>
+            <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-            <a:latin typeface="Times New Roman"/>
+            <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
           </a:endParaRPr>
         </a:p>
       </xdr:txBody>
@@ -10479,14 +10769,14 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>87840</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>88200</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>371520</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>100800</xdr:rowOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>59980</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -10501,8 +10791,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9871920" y="4820040"/>
-          <a:ext cx="4564080" cy="1940400"/>
+          <a:off x="10755840" y="5755821"/>
+          <a:ext cx="4950930" cy="2441230"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10534,7 +10824,8 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             </a:rPr>
             <a:t>　U1TOK ※通信開始のトリガー</a:t>
           </a:r>
@@ -10542,7 +10833,8 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             </a:rPr>
             <a:t>　　PID</a:t>
           </a:r>
@@ -10550,7 +10842,8 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             </a:rPr>
             <a:t>　　　1101:SETUP(TX)トークン</a:t>
           </a:r>
@@ -10558,7 +10851,8 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             </a:rPr>
             <a:t>　　　1001:IN(RX)トークン</a:t>
           </a:r>
@@ -10566,7 +10860,8 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             </a:rPr>
             <a:t>　　　0001:OUT(TX)トークン</a:t>
           </a:r>
@@ -10574,7 +10869,8 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             </a:rPr>
             <a:t>　　EP:通信するEPナンバーを指定</a:t>
           </a:r>
@@ -10582,7 +10878,8 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             </a:rPr>
             <a:t>　　　0000:EP0(SETUP)</a:t>
           </a:r>
@@ -10590,7 +10887,8 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             </a:rPr>
             <a:t>　　　0001:EP1(IN)</a:t>
           </a:r>
@@ -10598,7 +10896,8 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             </a:rPr>
             <a:t>　　　0002:EP2(OUT)</a:t>
           </a:r>
@@ -10609,16 +10908,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>87480</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>522909</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>24552</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>382320</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>100080</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>150999</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>149678</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -10633,8 +10932,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9871560" y="6873120"/>
-          <a:ext cx="4575240" cy="1464120"/>
+          <a:off x="5190159" y="11876373"/>
+          <a:ext cx="4962090" cy="2070948"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10666,7 +10965,8 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             </a:rPr>
             <a:t>　U1EP0</a:t>
           </a:r>
@@ -10674,7 +10974,8 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             </a:rPr>
             <a:t>　　LSPD=0,1:ロースピード無効(0)、有効(1)</a:t>
           </a:r>
@@ -10682,15 +10983,24 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             </a:rPr>
-            <a:t>　　BETRYDIS=1:NAKトランザクションのリトライ無効</a:t>
+            <a:t>　　BETRYDIS=1:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" strike="noStrike" spc="-1">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>NAKトランザクションのリトライ無効</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             </a:rPr>
             <a:t>　　EPRXEN=1:このU1EP0の受信を有効</a:t>
           </a:r>
@@ -10698,7 +11008,8 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             </a:rPr>
             <a:t>　　EPTXEN=1:このU1EP0の送信を有効</a:t>
           </a:r>
@@ -10706,14 +11017,23 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             </a:rPr>
-            <a:t>　　EPHSHK=1:自動ハンドシェイクを有効</a:t>
+            <a:t>　　EPHSHK=1:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" strike="noStrike" spc="-1">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>自動ハンドシェイクを有効</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-            <a:latin typeface="Times New Roman"/>
+            <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
           </a:endParaRPr>
         </a:p>
       </xdr:txBody>
@@ -10746,8 +11066,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2461193" y="5265758"/>
-          <a:ext cx="7235176" cy="2381964"/>
+          <a:off x="2450610" y="5280373"/>
+          <a:ext cx="7196370" cy="2389020"/>
           <a:chOff x="2450610" y="5122530"/>
           <a:chExt cx="7196370" cy="2312820"/>
         </a:xfrm>
@@ -10799,7 +11119,8 @@
           <a:p>
             <a:r>
               <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Times New Roman"/>
+                <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               </a:rPr>
               <a:t>　USBメモリ</a:t>
             </a:r>
@@ -10807,7 +11128,8 @@
           <a:p>
             <a:r>
               <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Times New Roman"/>
+                <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               </a:rPr>
               <a:t>　デバイス</a:t>
             </a:r>
@@ -10902,7 +11224,8 @@
           <a:p>
             <a:r>
               <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Times New Roman"/>
+                <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               </a:rPr>
               <a:t>　PIC</a:t>
             </a:r>
@@ -10910,7 +11233,8 @@
           <a:p>
             <a:r>
               <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Times New Roman"/>
+                <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               </a:rPr>
               <a:t>　USB</a:t>
             </a:r>
@@ -10918,7 +11242,8 @@
           <a:p>
             <a:r>
               <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Times New Roman"/>
+                <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               </a:rPr>
               <a:t>　モジュール</a:t>
             </a:r>
@@ -10971,7 +11296,8 @@
           <a:p>
             <a:r>
               <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Times New Roman"/>
+                <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               </a:rPr>
               <a:t>　EP0 (SETUP IN, OUT)</a:t>
             </a:r>
@@ -11064,7 +11390,8 @@
           <a:p>
             <a:r>
               <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Times New Roman"/>
+                <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               </a:rPr>
               <a:t>　EP1 (IN デバイス→ホスト)</a:t>
             </a:r>
@@ -11157,7 +11484,8 @@
           <a:p>
             <a:r>
               <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Times New Roman"/>
+                <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               </a:rPr>
               <a:t>　EP2 (OUT デバイス←ホスト)</a:t>
             </a:r>
@@ -11170,15 +11498,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>90720</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>66240</xdr:rowOff>
+      <xdr:colOff>104327</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>161490</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>393480</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>124920</xdr:rowOff>
+      <xdr:colOff>407087</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>136071</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -11193,17 +11521,17 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10758720" y="2606240"/>
-          <a:ext cx="4970010" cy="1752013"/>
+          <a:off x="10772327" y="3345561"/>
+          <a:ext cx="4970010" cy="2097296"/>
         </a:xfrm>
         <a:prstGeom prst="borderCallout2">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 10897"/>
-            <a:gd name="adj2" fmla="val -454"/>
-            <a:gd name="adj3" fmla="val 11504"/>
-            <a:gd name="adj4" fmla="val -33888"/>
-            <a:gd name="adj5" fmla="val 137277"/>
-            <a:gd name="adj6" fmla="val -34134"/>
+            <a:gd name="adj1" fmla="val 12195"/>
+            <a:gd name="adj2" fmla="val -180"/>
+            <a:gd name="adj3" fmla="val 12249"/>
+            <a:gd name="adj4" fmla="val -35805"/>
+            <a:gd name="adj5" fmla="val 102285"/>
+            <a:gd name="adj6" fmla="val -35777"/>
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
@@ -11232,13 +11560,22 @@
         <a:lstStyle/>
         <a:p>
           <a:endParaRPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-            <a:latin typeface="Times New Roman"/>
+            <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
           </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>　</a:t>
+          </a:r>
+          <a:r>
             <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             </a:rPr>
             <a:t>割り込み関係</a:t>
           </a:r>
@@ -11246,59 +11583,99 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             </a:rPr>
-            <a:t>　U1Ebits.ATTACHIE=1,0:Enable,disEnable ATTACH interrupt</a:t>
+            <a:t>　</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>　</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>U1Ebits.ATTACHIE=1,0:Enable,disEnable ATTACH interrupt</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             </a:rPr>
-            <a:t>　U1Ebits.DETACHIE=1,0:Enable,disEnable DETACH interrupt</a:t>
+            <a:t>　</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>　</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>U1Ebits.DETACHIE=1,0:Enable,disEnable DETACH interrupt</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             </a:rPr>
-            <a:t>　U1Ebits.SOFIE=1:Enable SOF interrupt</a:t>
+            <a:t>　</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>　</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>U1Ebits.SOFIE=1:Enable SOF interrupt</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             </a:rPr>
-            <a:t>　U1EIE:Enable All Error Interrupts </a:t>
+            <a:t>　</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>　</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>U1EIE:Enable All Error Interrupts </a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>その他</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>　U1CONbits.SOFEN=1:SOF packet の自動1ms送信スタート</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-            <a:latin typeface="Times New Roman"/>
+            <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
           </a:endParaRPr>
         </a:p>
       </xdr:txBody>
@@ -11315,8 +11692,8 @@
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>388620</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>159717</xdr:rowOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>149678</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -11331,8 +11708,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="10814444" y="8540750"/>
-          <a:ext cx="7671676" cy="3966189"/>
+          <a:off x="10758000" y="8564940"/>
+          <a:ext cx="7632870" cy="5382381"/>
           <a:chOff x="10814444" y="8540750"/>
           <a:chExt cx="7671676" cy="3966189"/>
         </a:xfrm>
@@ -11383,20 +11760,23 @@
           <a:p>
             <a:r>
               <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Times New Roman"/>
+                <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               </a:rPr>
               <a:t>　BDT0 (EP0_RX, IN)</a:t>
             </a:r>
           </a:p>
           <a:p>
             <a:endParaRPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             </a:endParaRPr>
           </a:p>
           <a:p>
             <a:r>
               <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Times New Roman"/>
+                <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               </a:rPr>
               <a:t>　　UOWN=1:USBモジュールが制御 0:ソフトウェアが制御</a:t>
             </a:r>
@@ -11404,7 +11784,8 @@
           <a:p>
             <a:r>
               <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Times New Roman"/>
+                <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               </a:rPr>
               <a:t>　　DTS=0:DATA0/1:DATA1</a:t>
             </a:r>
@@ -11412,40 +11793,46 @@
           <a:p>
             <a:r>
               <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Times New Roman"/>
+                <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               </a:rPr>
               <a:t>　　COUNTER:送受信バイト数</a:t>
             </a:r>
           </a:p>
           <a:p>
             <a:endParaRPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             </a:endParaRPr>
           </a:p>
           <a:p>
             <a:r>
               <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Times New Roman"/>
+                <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               </a:rPr>
               <a:t>　　ADDRESS:バッファアドレス(DMA転送元先)</a:t>
             </a:r>
           </a:p>
           <a:p>
             <a:endParaRPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             </a:endParaRPr>
           </a:p>
           <a:p>
             <a:r>
               <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Times New Roman"/>
+                <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               </a:rPr>
               <a:t>　　PID:ハンドシェイクのPIDがリターン</a:t>
             </a:r>
           </a:p>
           <a:p>
             <a:endParaRPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -11496,20 +11883,23 @@
           <a:p>
             <a:r>
               <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Times New Roman"/>
+                <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               </a:rPr>
               <a:t>　BDT1 (EP0_TX, OUT)</a:t>
             </a:r>
           </a:p>
           <a:p>
             <a:endParaRPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             </a:endParaRPr>
           </a:p>
           <a:p>
             <a:r>
               <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Times New Roman"/>
+                <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               </a:rPr>
               <a:t>　　UOWN=1:USBモジュールが制御 0:ソフトウェアが制御</a:t>
             </a:r>
@@ -11517,7 +11907,8 @@
           <a:p>
             <a:r>
               <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Times New Roman"/>
+                <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               </a:rPr>
               <a:t>　　DTS=0:DATA0/1:DATA1</a:t>
             </a:r>
@@ -11525,40 +11916,46 @@
           <a:p>
             <a:r>
               <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Times New Roman"/>
+                <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               </a:rPr>
               <a:t>　　COUNTER:送受信バイト数</a:t>
             </a:r>
           </a:p>
           <a:p>
             <a:endParaRPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             </a:endParaRPr>
           </a:p>
           <a:p>
             <a:r>
               <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Times New Roman"/>
+                <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               </a:rPr>
               <a:t>　　ADDRESS:バッファアドレス(DMA転送元先)</a:t>
             </a:r>
           </a:p>
           <a:p>
             <a:endParaRPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             </a:endParaRPr>
           </a:p>
           <a:p>
             <a:r>
               <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Times New Roman"/>
+                <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               </a:rPr>
               <a:t>　　PID:ハンドシェイクのPIDがリターン</a:t>
             </a:r>
           </a:p>
           <a:p>
             <a:endParaRPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:latin typeface="Times New Roman"/>
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -11609,7 +12006,8 @@
           <a:p>
             <a:r>
               <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Times New Roman"/>
+                <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               </a:rPr>
               <a:t>　DATA buffer</a:t>
             </a:r>
@@ -11742,7 +12140,8 @@
           <a:p>
             <a:r>
               <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Times New Roman"/>
+                <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
               </a:rPr>
               <a:t>　DATA buffer</a:t>
             </a:r>
@@ -11755,15 +12154,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>188149</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>23519</xdr:rowOff>
+      <xdr:colOff>174542</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>91554</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>188149</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>152872</xdr:rowOff>
+      <xdr:colOff>174542</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>44014</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -11778,8 +12177,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16274816" y="8666575"/>
-          <a:ext cx="2681111" cy="834908"/>
+          <a:off x="16176542" y="8936197"/>
+          <a:ext cx="2667000" cy="836924"/>
         </a:xfrm>
         <a:prstGeom prst="borderCallout1">
           <a:avLst>
@@ -11812,31 +12211,52 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1200">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            </a:rPr>
             <a:t> </a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1200">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            </a:rPr>
             <a:t>DATA0/1</a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1200">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            </a:rPr>
             <a:t>は、通信しているそれぞれの</a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1200">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            </a:rPr>
             <a:t>EP0,EP1,EP2 </a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1200">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            </a:rPr>
             <a:t>ごとに、</a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1200">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            </a:rPr>
             <a:t>0,1</a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1200">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            </a:rPr>
             <a:t>をフリップフロップする必要あり</a:t>
           </a:r>
         </a:p>
@@ -11846,23 +12266,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>175920</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>58327</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>163286</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>55774</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>175920</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>11290</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>7727</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>8737</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="23" name="線吹き出し 1 (枠付き) 22">
+        <xdr:cNvPr id="24" name="線吹き出し 1 (枠付き) 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000017000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11870,15 +12290,15 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16262587" y="10641660"/>
-          <a:ext cx="2681111" cy="834908"/>
+          <a:off x="6830786" y="8015953"/>
+          <a:ext cx="3178191" cy="837427"/>
         </a:xfrm>
         <a:prstGeom prst="borderCallout1">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 46918"/>
-            <a:gd name="adj2" fmla="val -438"/>
-            <a:gd name="adj3" fmla="val 70247"/>
-            <a:gd name="adj4" fmla="val -123859"/>
+            <a:gd name="adj1" fmla="val 1848"/>
+            <a:gd name="adj2" fmla="val 99123"/>
+            <a:gd name="adj3" fmla="val 83738"/>
+            <a:gd name="adj4" fmla="val 127295"/>
           </a:avLst>
         </a:prstGeom>
       </xdr:spPr>
@@ -11904,33 +12324,44 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1200">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            </a:rPr>
             <a:t> </a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
-            <a:t>DATA0/1</a:t>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1200">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>BDT</a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>は、通信しているそれぞれの</a:t>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1200">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>テーブルの開始位置は、メモリアドレスの</a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
-            <a:t>EP0,EP1,EP2 </a:t>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1200">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>512BYTE</a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>ごとに、</a:t>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1200">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>境界に合わせる必要あり。</a:t>
           </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
-            <a:t>0,1</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>をフリップフロップする必要あり</a:t>
-          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1200">
+            <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -11938,23 +12369,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>470370</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>164630</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>321904</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>9440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>470370</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>117593</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>321904</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>138793</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="24" name="線吹き出し 1 (枠付き) 23">
+        <xdr:cNvPr id="25" name="線吹き出し 1 (枠付き) 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11962,15 +12393,15 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7843426" y="10571574"/>
-          <a:ext cx="2681111" cy="834908"/>
+          <a:off x="2322154" y="11861261"/>
+          <a:ext cx="2667000" cy="836925"/>
         </a:xfrm>
         <a:prstGeom prst="borderCallout1">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 1848"/>
-            <a:gd name="adj2" fmla="val 99123"/>
-            <a:gd name="adj3" fmla="val -239612"/>
-            <a:gd name="adj4" fmla="val 111667"/>
+            <a:gd name="adj1" fmla="val 4645"/>
+            <a:gd name="adj2" fmla="val 100072"/>
+            <a:gd name="adj3" fmla="val 31906"/>
+            <a:gd name="adj4" fmla="val 113036"/>
           </a:avLst>
         </a:prstGeom>
       </xdr:spPr>
@@ -11996,101 +12427,25 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
-            <a:t>BDT</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>テーブルの開始位置は、メモリアドレスの</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
-            <a:t>512BYTE</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>境界に合わせるひつよう必要あり。</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>199438</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>23048</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>199438</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>152401</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="25" name="線吹き出し 1 (枠付き) 24">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000019000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="16286105" y="6902215"/>
-          <a:ext cx="2681111" cy="834908"/>
-        </a:xfrm>
-        <a:prstGeom prst="borderCallout1">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 46918"/>
-            <a:gd name="adj2" fmla="val -438"/>
-            <a:gd name="adj3" fmla="val 2641"/>
-            <a:gd name="adj4" fmla="val -18596"/>
-          </a:avLst>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1200">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            </a:rPr>
             <a:t> ホストモードでは、</a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1200">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            </a:rPr>
             <a:t>U1EP0</a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>のレジスタのみ実行。</a:t>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1200">
+              <a:latin typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="游ゴシック Medium" panose="020B0500000000000000" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>のレジスタのみ使用。</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -12100,15 +12455,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>376297</xdr:colOff>
+      <xdr:colOff>585107</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>82314</xdr:rowOff>
+      <xdr:rowOff>82313</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>258704</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>84550</xdr:rowOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>108857</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -12123,8 +12478,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="8419630" y="8725370"/>
-          <a:ext cx="2563518" cy="884180"/>
+          <a:off x="8586107" y="8750063"/>
+          <a:ext cx="2340597" cy="1972365"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -14867,7 +15222,7 @@
   </sheetPr>
   <dimension ref="A1:AMK54"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="V54" sqref="V54"/>
     </sheetView>
   </sheetViews>
@@ -15802,13 +16157,13 @@
       <c r="P26" s="30" t="s">
         <v>181</v>
       </c>
-      <c r="Q26" s="98" t="s">
+      <c r="Q26" s="103" t="s">
         <v>182</v>
       </c>
-      <c r="R26" s="98"/>
-      <c r="S26" s="98"/>
-      <c r="T26" s="98"/>
-      <c r="U26" s="98"/>
+      <c r="R26" s="103"/>
+      <c r="S26" s="103"/>
+      <c r="T26" s="103"/>
+      <c r="U26" s="103"/>
       <c r="V26" s="33" t="s">
         <v>183</v>
       </c>
@@ -15836,13 +16191,13 @@
       <c r="P27" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="Q27" s="99" t="s">
+      <c r="Q27" s="104" t="s">
         <v>23</v>
       </c>
-      <c r="R27" s="99"/>
-      <c r="S27" s="99"/>
-      <c r="T27" s="99"/>
-      <c r="U27" s="99"/>
+      <c r="R27" s="104"/>
+      <c r="S27" s="104"/>
+      <c r="T27" s="104"/>
+      <c r="U27" s="104"/>
       <c r="V27" s="38" t="str">
         <f t="shared" ref="V27:V40" si="0">B10</f>
         <v>10K</v>
@@ -15891,11 +16246,11 @@
       <c r="N28" s="40"/>
       <c r="O28" s="41"/>
       <c r="P28" s="42"/>
-      <c r="Q28" s="100"/>
-      <c r="R28" s="100"/>
-      <c r="S28" s="100"/>
-      <c r="T28" s="100"/>
-      <c r="U28" s="100"/>
+      <c r="Q28" s="105"/>
+      <c r="R28" s="105"/>
+      <c r="S28" s="105"/>
+      <c r="T28" s="105"/>
+      <c r="U28" s="105"/>
       <c r="V28" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -15944,11 +16299,11 @@
       <c r="N29" s="40"/>
       <c r="O29" s="41"/>
       <c r="P29" s="42"/>
-      <c r="Q29" s="100"/>
-      <c r="R29" s="100"/>
-      <c r="S29" s="100"/>
-      <c r="T29" s="100"/>
-      <c r="U29" s="100"/>
+      <c r="Q29" s="105"/>
+      <c r="R29" s="105"/>
+      <c r="S29" s="105"/>
+      <c r="T29" s="105"/>
+      <c r="U29" s="105"/>
       <c r="V29" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -15991,13 +16346,13 @@
       <c r="P30" s="42" t="s">
         <v>185</v>
       </c>
-      <c r="Q30" s="100" t="s">
+      <c r="Q30" s="105" t="s">
         <v>186</v>
       </c>
-      <c r="R30" s="100"/>
-      <c r="S30" s="100"/>
-      <c r="T30" s="100"/>
-      <c r="U30" s="100"/>
+      <c r="R30" s="105"/>
+      <c r="S30" s="105"/>
+      <c r="T30" s="105"/>
+      <c r="U30" s="105"/>
       <c r="V30" s="43" t="str">
         <f t="shared" si="0"/>
         <v>PGD1</v>
@@ -16040,13 +16395,13 @@
       <c r="P31" s="42" t="s">
         <v>185</v>
       </c>
-      <c r="Q31" s="100" t="s">
+      <c r="Q31" s="105" t="s">
         <v>187</v>
       </c>
-      <c r="R31" s="100"/>
-      <c r="S31" s="100"/>
-      <c r="T31" s="100"/>
-      <c r="U31" s="100"/>
+      <c r="R31" s="105"/>
+      <c r="S31" s="105"/>
+      <c r="T31" s="105"/>
+      <c r="U31" s="105"/>
       <c r="V31" s="43" t="str">
         <f t="shared" si="0"/>
         <v>PGC1</v>
@@ -16087,11 +16442,11 @@
       <c r="N32" s="40"/>
       <c r="O32" s="41"/>
       <c r="P32" s="42"/>
-      <c r="Q32" s="100"/>
-      <c r="R32" s="100"/>
-      <c r="S32" s="100"/>
-      <c r="T32" s="100"/>
-      <c r="U32" s="100"/>
+      <c r="Q32" s="105"/>
+      <c r="R32" s="105"/>
+      <c r="S32" s="105"/>
+      <c r="T32" s="105"/>
+      <c r="U32" s="105"/>
       <c r="V32" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -16134,11 +16489,11 @@
       <c r="N33" s="40"/>
       <c r="O33" s="41"/>
       <c r="P33" s="42"/>
-      <c r="Q33" s="100"/>
-      <c r="R33" s="100"/>
-      <c r="S33" s="100"/>
-      <c r="T33" s="100"/>
-      <c r="U33" s="100"/>
+      <c r="Q33" s="105"/>
+      <c r="R33" s="105"/>
+      <c r="S33" s="105"/>
+      <c r="T33" s="105"/>
+      <c r="U33" s="105"/>
       <c r="V33" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -16167,13 +16522,13 @@
       <c r="P34" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="Q34" s="99" t="s">
+      <c r="Q34" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="R34" s="99"/>
-      <c r="S34" s="99"/>
-      <c r="T34" s="99"/>
-      <c r="U34" s="99"/>
+      <c r="R34" s="104"/>
+      <c r="S34" s="104"/>
+      <c r="T34" s="104"/>
+      <c r="U34" s="104"/>
       <c r="V34" s="38" t="str">
         <f t="shared" si="0"/>
         <v>GND</v>
@@ -16210,13 +16565,13 @@
       <c r="N35" s="40"/>
       <c r="O35" s="41"/>
       <c r="P35" s="42"/>
-      <c r="Q35" s="100" t="s">
+      <c r="Q35" s="105" t="s">
         <v>188</v>
       </c>
-      <c r="R35" s="100"/>
-      <c r="S35" s="100"/>
-      <c r="T35" s="100"/>
-      <c r="U35" s="100"/>
+      <c r="R35" s="105"/>
+      <c r="S35" s="105"/>
+      <c r="T35" s="105"/>
+      <c r="U35" s="105"/>
       <c r="V35" s="43" t="str">
         <f t="shared" si="0"/>
         <v>OSCI</v>
@@ -16251,13 +16606,13 @@
       <c r="N36" s="40"/>
       <c r="O36" s="41"/>
       <c r="P36" s="42"/>
-      <c r="Q36" s="100" t="s">
+      <c r="Q36" s="105" t="s">
         <v>188</v>
       </c>
-      <c r="R36" s="100"/>
-      <c r="S36" s="100"/>
-      <c r="T36" s="100"/>
-      <c r="U36" s="100"/>
+      <c r="R36" s="105"/>
+      <c r="S36" s="105"/>
+      <c r="T36" s="105"/>
+      <c r="U36" s="105"/>
       <c r="V36" s="43" t="str">
         <f t="shared" si="0"/>
         <v>OSCO</v>
@@ -16294,13 +16649,13 @@
       <c r="N37" s="40"/>
       <c r="O37" s="41"/>
       <c r="P37" s="42"/>
-      <c r="Q37" s="100" t="s">
+      <c r="Q37" s="105" t="s">
         <v>105</v>
       </c>
-      <c r="R37" s="100"/>
-      <c r="S37" s="100"/>
-      <c r="T37" s="100"/>
-      <c r="U37" s="100"/>
+      <c r="R37" s="105"/>
+      <c r="S37" s="105"/>
+      <c r="T37" s="105"/>
+      <c r="U37" s="105"/>
       <c r="V37" s="43" t="str">
         <f t="shared" si="0"/>
         <v>SOSCI</v>
@@ -16339,13 +16694,13 @@
       <c r="N38" s="40"/>
       <c r="O38" s="41"/>
       <c r="P38" s="42"/>
-      <c r="Q38" s="100" t="s">
+      <c r="Q38" s="105" t="s">
         <v>105</v>
       </c>
-      <c r="R38" s="100"/>
-      <c r="S38" s="100"/>
-      <c r="T38" s="100"/>
-      <c r="U38" s="100"/>
+      <c r="R38" s="105"/>
+      <c r="S38" s="105"/>
+      <c r="T38" s="105"/>
+      <c r="U38" s="105"/>
       <c r="V38" s="43" t="str">
         <f t="shared" si="0"/>
         <v>SOSCO</v>
@@ -16374,11 +16729,11 @@
       <c r="P39" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="Q39" s="99"/>
-      <c r="R39" s="99"/>
-      <c r="S39" s="99"/>
-      <c r="T39" s="99"/>
-      <c r="U39" s="99"/>
+      <c r="Q39" s="104"/>
+      <c r="R39" s="104"/>
+      <c r="S39" s="104"/>
+      <c r="T39" s="104"/>
+      <c r="U39" s="104"/>
       <c r="V39" s="38" t="str">
         <f t="shared" si="0"/>
         <v>+3.3V</v>
@@ -16411,13 +16766,13 @@
       <c r="N40" s="40"/>
       <c r="O40" s="41"/>
       <c r="P40" s="42"/>
-      <c r="Q40" s="100" t="s">
+      <c r="Q40" s="105" t="s">
         <v>178</v>
       </c>
-      <c r="R40" s="100"/>
-      <c r="S40" s="100"/>
-      <c r="T40" s="100"/>
-      <c r="U40" s="100"/>
+      <c r="R40" s="105"/>
+      <c r="S40" s="105"/>
+      <c r="T40" s="105"/>
+      <c r="U40" s="105"/>
       <c r="V40" s="43" t="str">
         <f t="shared" si="0"/>
         <v>LED1</v>
@@ -16446,11 +16801,11 @@
       <c r="P41" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="Q41" s="99"/>
-      <c r="R41" s="99"/>
-      <c r="S41" s="99"/>
-      <c r="T41" s="99"/>
-      <c r="U41" s="99"/>
+      <c r="Q41" s="104"/>
+      <c r="R41" s="104"/>
+      <c r="S41" s="104"/>
+      <c r="T41" s="104"/>
+      <c r="U41" s="104"/>
       <c r="V41" s="38" t="str">
         <f>Z23</f>
         <v>VBUS</v>
@@ -16487,11 +16842,11 @@
       <c r="N42" s="40"/>
       <c r="O42" s="41"/>
       <c r="P42" s="42"/>
-      <c r="Q42" s="100"/>
-      <c r="R42" s="100"/>
-      <c r="S42" s="100"/>
-      <c r="T42" s="100"/>
-      <c r="U42" s="100"/>
+      <c r="Q42" s="105"/>
+      <c r="R42" s="105"/>
+      <c r="S42" s="105"/>
+      <c r="T42" s="105"/>
+      <c r="U42" s="105"/>
       <c r="V42" s="43">
         <f>Z22</f>
         <v>0</v>
@@ -16532,13 +16887,13 @@
       <c r="P43" s="42" t="s">
         <v>189</v>
       </c>
-      <c r="Q43" s="100" t="s">
+      <c r="Q43" s="105" t="s">
         <v>190</v>
       </c>
-      <c r="R43" s="100"/>
-      <c r="S43" s="100"/>
-      <c r="T43" s="100"/>
-      <c r="U43" s="100"/>
+      <c r="R43" s="105"/>
+      <c r="S43" s="105"/>
+      <c r="T43" s="105"/>
+      <c r="U43" s="105"/>
       <c r="V43" s="43" t="str">
         <f>Z21</f>
         <v>TX(→RX)</v>
@@ -16579,13 +16934,13 @@
       <c r="P44" s="42" t="s">
         <v>191</v>
       </c>
-      <c r="Q44" s="100" t="s">
+      <c r="Q44" s="105" t="s">
         <v>190</v>
       </c>
-      <c r="R44" s="100"/>
-      <c r="S44" s="100"/>
-      <c r="T44" s="100"/>
-      <c r="U44" s="100"/>
+      <c r="R44" s="105"/>
+      <c r="S44" s="105"/>
+      <c r="T44" s="105"/>
+      <c r="U44" s="105"/>
       <c r="V44" s="43" t="str">
         <f>Z20</f>
         <v>RX(→TX)</v>
@@ -16614,13 +16969,13 @@
       <c r="P45" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="Q45" s="99" t="s">
+      <c r="Q45" s="104" t="s">
         <v>192</v>
       </c>
-      <c r="R45" s="99"/>
-      <c r="S45" s="99"/>
-      <c r="T45" s="99"/>
-      <c r="U45" s="99"/>
+      <c r="R45" s="104"/>
+      <c r="S45" s="104"/>
+      <c r="T45" s="104"/>
+      <c r="U45" s="104"/>
       <c r="V45" s="38" t="str">
         <f>Z19</f>
         <v>GND</v>
@@ -16651,13 +17006,13 @@
       <c r="P46" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="Q46" s="99" t="s">
+      <c r="Q46" s="104" t="s">
         <v>193</v>
       </c>
-      <c r="R46" s="99"/>
-      <c r="S46" s="99"/>
-      <c r="T46" s="99"/>
-      <c r="U46" s="99"/>
+      <c r="R46" s="104"/>
+      <c r="S46" s="104"/>
+      <c r="T46" s="104"/>
+      <c r="U46" s="104"/>
       <c r="V46" s="38" t="str">
         <f>Z18</f>
         <v>10uF</v>
@@ -16741,13 +17096,13 @@
       <c r="P48" s="42" t="s">
         <v>181</v>
       </c>
-      <c r="Q48" s="100" t="s">
+      <c r="Q48" s="105" t="s">
         <v>194</v>
       </c>
-      <c r="R48" s="100"/>
-      <c r="S48" s="100"/>
-      <c r="T48" s="100"/>
-      <c r="U48" s="100"/>
+      <c r="R48" s="105"/>
+      <c r="S48" s="105"/>
+      <c r="T48" s="105"/>
+      <c r="U48" s="105"/>
       <c r="V48" s="43" t="str">
         <f>Z16</f>
         <v>D-(→D+)</v>
@@ -16776,11 +17131,11 @@
       <c r="P49" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="Q49" s="99"/>
-      <c r="R49" s="99"/>
-      <c r="S49" s="99"/>
-      <c r="T49" s="99"/>
-      <c r="U49" s="99"/>
+      <c r="Q49" s="104"/>
+      <c r="R49" s="104"/>
+      <c r="S49" s="104"/>
+      <c r="T49" s="104"/>
+      <c r="U49" s="104"/>
       <c r="V49" s="38" t="str">
         <f>Z15</f>
         <v>+3.3V</v>
@@ -16821,11 +17176,11 @@
       <c r="N50" s="40"/>
       <c r="O50" s="41"/>
       <c r="P50" s="42"/>
-      <c r="Q50" s="100"/>
-      <c r="R50" s="100"/>
-      <c r="S50" s="100"/>
-      <c r="T50" s="100"/>
-      <c r="U50" s="100"/>
+      <c r="Q50" s="105"/>
+      <c r="R50" s="105"/>
+      <c r="S50" s="105"/>
+      <c r="T50" s="105"/>
+      <c r="U50" s="105"/>
       <c r="V50" s="43">
         <f>Z14</f>
         <v>0</v>
@@ -16866,11 +17221,11 @@
       <c r="N51" s="40"/>
       <c r="O51" s="41"/>
       <c r="P51" s="42"/>
-      <c r="Q51" s="100"/>
-      <c r="R51" s="100"/>
-      <c r="S51" s="100"/>
-      <c r="T51" s="100"/>
-      <c r="U51" s="100"/>
+      <c r="Q51" s="105"/>
+      <c r="R51" s="105"/>
+      <c r="S51" s="105"/>
+      <c r="T51" s="105"/>
+      <c r="U51" s="105"/>
       <c r="V51" s="43">
         <f>Z13</f>
         <v>0</v>
@@ -16909,11 +17264,11 @@
       <c r="N52" s="40"/>
       <c r="O52" s="41"/>
       <c r="P52" s="42"/>
-      <c r="Q52" s="100"/>
-      <c r="R52" s="100"/>
-      <c r="S52" s="100"/>
-      <c r="T52" s="100"/>
-      <c r="U52" s="100"/>
+      <c r="Q52" s="105"/>
+      <c r="R52" s="105"/>
+      <c r="S52" s="105"/>
+      <c r="T52" s="105"/>
+      <c r="U52" s="105"/>
       <c r="V52" s="43">
         <f>Z12</f>
         <v>0</v>
@@ -16942,13 +17297,13 @@
       <c r="P53" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="Q53" s="99" t="s">
+      <c r="Q53" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="R53" s="99"/>
-      <c r="S53" s="99"/>
-      <c r="T53" s="99"/>
-      <c r="U53" s="99"/>
+      <c r="R53" s="104"/>
+      <c r="S53" s="104"/>
+      <c r="T53" s="104"/>
+      <c r="U53" s="104"/>
       <c r="V53" s="38" t="str">
         <f>Z11</f>
         <v>GND</v>
@@ -16977,13 +17332,13 @@
       <c r="P54" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="Q54" s="99" t="s">
+      <c r="Q54" s="104" t="s">
         <v>25</v>
       </c>
-      <c r="R54" s="99"/>
-      <c r="S54" s="99"/>
-      <c r="T54" s="99"/>
-      <c r="U54" s="99"/>
+      <c r="R54" s="104"/>
+      <c r="S54" s="104"/>
+      <c r="T54" s="104"/>
+      <c r="U54" s="104"/>
       <c r="V54" s="38" t="str">
         <f>Z10</f>
         <v>+3.3V</v>
@@ -19317,8 +19672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -21144,91 +21499,334 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A78:AMK88"/>
+  <dimension ref="A93:AMK144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H27" zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I63" sqref="I63"/>
+    <sheetView topLeftCell="A26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AD48" sqref="AD48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1025" width="8.75" style="72" customWidth="1"/>
+    <col min="1" max="1025" width="8.75" style="66" customWidth="1"/>
+    <col min="1026" max="16384" width="9" style="68"/>
   </cols>
   <sheetData>
-    <row r="78" spans="5:6" x14ac:dyDescent="0.15">
-      <c r="E78" s="72" t="s">
+    <row r="93" spans="5:6" x14ac:dyDescent="0.15">
+      <c r="E93" s="73" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="79" spans="5:6" x14ac:dyDescent="0.15">
-      <c r="E79" s="72" t="s">
+    <row r="94" spans="5:6" x14ac:dyDescent="0.15">
+      <c r="E94" s="66" t="s">
         <v>938</v>
       </c>
     </row>
-    <row r="80" spans="5:6" x14ac:dyDescent="0.15">
-      <c r="E80" s="72">
+    <row r="95" spans="5:6" x14ac:dyDescent="0.15">
+      <c r="E95" s="66">
         <v>44.3</v>
       </c>
-      <c r="F80" s="72" t="s">
+      <c r="F95" s="66" t="s">
         <v>939</v>
       </c>
     </row>
-    <row r="81" spans="5:6" x14ac:dyDescent="0.15">
-      <c r="E81" s="72">
-        <f>E80*1000</f>
+    <row r="96" spans="5:6" x14ac:dyDescent="0.15">
+      <c r="E96" s="66">
+        <f>E95*1000</f>
         <v>44300</v>
       </c>
-      <c r="F81" s="72" t="s">
+      <c r="F96" s="66" t="s">
         <v>940</v>
       </c>
     </row>
-    <row r="82" spans="5:6" x14ac:dyDescent="0.15">
-      <c r="E82" s="72">
-        <f>E81*2*2</f>
+    <row r="97" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="E97" s="66">
+        <f>E96*2*2</f>
         <v>177200</v>
       </c>
-      <c r="F82" s="72" t="s">
+      <c r="F97" s="66" t="s">
         <v>941</v>
       </c>
     </row>
-    <row r="83" spans="5:6" x14ac:dyDescent="0.15">
-      <c r="E83" s="72">
-        <f>E82/1000</f>
+    <row r="98" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="E98" s="66">
+        <f>E97/1000</f>
         <v>177.2</v>
       </c>
-      <c r="F83" s="72" t="s">
+      <c r="F98" s="66" t="s">
         <v>942</v>
       </c>
     </row>
-    <row r="85" spans="5:6" x14ac:dyDescent="0.15">
-      <c r="E85" s="72" t="s">
+    <row r="100" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="E100" s="66" t="s">
         <v>943</v>
       </c>
     </row>
-    <row r="86" spans="5:6" x14ac:dyDescent="0.15">
-      <c r="E86" s="72">
+    <row r="101" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="E101" s="66">
         <v>12</v>
       </c>
-      <c r="F86" s="72" t="s">
+      <c r="F101" s="66" t="s">
         <v>944</v>
       </c>
     </row>
-    <row r="87" spans="5:6" x14ac:dyDescent="0.15">
-      <c r="E87" s="72">
-        <f>E86*1000000</f>
+    <row r="102" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="E102" s="66">
+        <f>E101*1000000</f>
         <v>12000000</v>
       </c>
-      <c r="F87" s="72" t="s">
+      <c r="F102" s="66" t="s">
         <v>945</v>
       </c>
     </row>
-    <row r="88" spans="5:6" x14ac:dyDescent="0.15">
-      <c r="E88" s="72">
-        <f>E87/1000/8</f>
+    <row r="103" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="E103" s="66">
+        <f>E102/1000/8</f>
         <v>1500</v>
       </c>
-      <c r="F88" s="72" t="s">
+      <c r="F103" s="66" t="s">
         <v>942</v>
+      </c>
+    </row>
+    <row r="108" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="E108" s="73" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="109" spans="5:14" ht="22.5" x14ac:dyDescent="0.15">
+      <c r="F109" s="98" t="s">
+        <v>956</v>
+      </c>
+      <c r="G109" s="99" t="s">
+        <v>957</v>
+      </c>
+      <c r="H109" s="100" t="s">
+        <v>958</v>
+      </c>
+      <c r="I109" s="101"/>
+      <c r="J109" s="100" t="s">
+        <v>959</v>
+      </c>
+      <c r="K109" s="101"/>
+      <c r="L109" s="100" t="s">
+        <v>960</v>
+      </c>
+      <c r="M109" s="101"/>
+      <c r="N109" s="66" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="110" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="E110" s="102" t="s">
+        <v>946</v>
+      </c>
+      <c r="F110" s="66" t="s">
+        <v>947</v>
+      </c>
+      <c r="G110" s="66" t="s">
+        <v>948</v>
+      </c>
+      <c r="H110" s="76" t="s">
+        <v>949</v>
+      </c>
+      <c r="I110" s="66" t="s">
+        <v>950</v>
+      </c>
+      <c r="J110" s="66" t="s">
+        <v>950</v>
+      </c>
+      <c r="K110" s="66" t="s">
+        <v>950</v>
+      </c>
+      <c r="L110" s="66" t="s">
+        <v>950</v>
+      </c>
+      <c r="M110" s="66" t="s">
+        <v>951</v>
+      </c>
+      <c r="N110" s="66" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="112" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="E112" s="73" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="113" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="E113" s="102" t="s">
+        <v>946</v>
+      </c>
+      <c r="F113" s="66" t="s">
+        <v>947</v>
+      </c>
+      <c r="G113" s="66" t="s">
+        <v>953</v>
+      </c>
+      <c r="H113" s="76" t="s">
+        <v>949</v>
+      </c>
+      <c r="I113" s="66" t="s">
+        <v>950</v>
+      </c>
+      <c r="J113" s="66" t="s">
+        <v>950</v>
+      </c>
+      <c r="K113" s="66" t="s">
+        <v>950</v>
+      </c>
+      <c r="L113" s="66" t="s">
+        <v>950</v>
+      </c>
+      <c r="M113" s="66" t="s">
+        <v>951</v>
+      </c>
+      <c r="N113" s="66" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="116" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="E116" s="66" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="117" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="F117" s="66" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="118" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="G118" s="73" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="119" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="G119" s="66" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="120" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="F120" s="66" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="121" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="G121" s="73" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="122" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="G122" s="66" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="123" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="G123" s="66" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="124" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="G124" s="66" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="125" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="F125" s="66" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="126" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="G126" s="73" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="127" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="G127" s="66" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="128" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="G128" s="66" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="129" spans="5:7" x14ac:dyDescent="0.15">
+      <c r="G129" s="66" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="130" spans="5:7" x14ac:dyDescent="0.15">
+      <c r="G130" s="66" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="131" spans="5:7" x14ac:dyDescent="0.15">
+      <c r="E131" s="66" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="132" spans="5:7" x14ac:dyDescent="0.15">
+      <c r="F132" s="66" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="133" spans="5:7" x14ac:dyDescent="0.15">
+      <c r="F133" s="66" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="134" spans="5:7" x14ac:dyDescent="0.15">
+      <c r="F134" s="66" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="135" spans="5:7" x14ac:dyDescent="0.15">
+      <c r="F135" s="66" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="136" spans="5:7" x14ac:dyDescent="0.15">
+      <c r="F136" s="66" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="137" spans="5:7" x14ac:dyDescent="0.15">
+      <c r="F137" s="73" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="138" spans="5:7" x14ac:dyDescent="0.15">
+      <c r="F138" s="66" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="139" spans="5:7" x14ac:dyDescent="0.15">
+      <c r="F139" s="66" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="140" spans="5:7" x14ac:dyDescent="0.15">
+      <c r="F140" s="66" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="141" spans="5:7" x14ac:dyDescent="0.15">
+      <c r="F141" s="73" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="142" spans="5:7" x14ac:dyDescent="0.15">
+      <c r="F142" s="66" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="143" spans="5:7" x14ac:dyDescent="0.15">
+      <c r="F143" s="66" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="144" spans="5:7" x14ac:dyDescent="0.15">
+      <c r="F144" s="66" t="s">
+        <v>990</v>
       </c>
     </row>
   </sheetData>

</xml_diff>